<commit_message>
Modify sample_questions with actual questions
</commit_message>
<xml_diff>
--- a/prototype/sample_questions.xlsx
+++ b/prototype/sample_questions.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ca35025d8a608f25/Documents/cs3103/project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ca35025d8a608f25/Documents/cs3103proj_exam/prototype/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="14" documentId="8_{3911BD6C-A5DC-4653-B6C0-B36186FF75DF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{7F0FA3BB-154F-4FBD-A645-B8993B3B3C49}"/>
+  <xr:revisionPtr revIDLastSave="99" documentId="8_{3911BD6C-A5DC-4653-B6C0-B36186FF75DF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{832D4618-BC5D-4578-AAA6-C7B709B400C5}"/>
   <bookViews>
-    <workbookView xWindow="3996" yWindow="60" windowWidth="17280" windowHeight="11052" xr2:uid="{B39240BB-16A0-4C86-9AA4-FBD9078AD770}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B39240BB-16A0-4C86-9AA4-FBD9078AD770}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="52">
   <si>
     <t>No.</t>
   </si>
@@ -52,13 +52,145 @@
     <t>MCQ</t>
   </si>
   <si>
-    <t>exam duration</t>
-  </si>
-  <si>
-    <t>question 1</t>
-  </si>
-  <si>
-    <t>question 2</t>
+    <t>As compared to its parent alkane, an alkyl radical contains one</t>
+  </si>
+  <si>
+    <t>The rate of reaction of organic compounds is slow due to</t>
+  </si>
+  <si>
+    <t>less hydrogen</t>
+  </si>
+  <si>
+    <t>less carbon</t>
+  </si>
+  <si>
+    <t>more carbon</t>
+  </si>
+  <si>
+    <t>more hydrogen</t>
+  </si>
+  <si>
+    <t>ionic bonding</t>
+  </si>
+  <si>
+    <t>amphoteric nature</t>
+  </si>
+  <si>
+    <t>covalent bonding</t>
+  </si>
+  <si>
+    <t>coordinate covalent bonding</t>
+  </si>
+  <si>
+    <t>In naming alkane the stem tells about the number of</t>
+  </si>
+  <si>
+    <t>hydrogen atoms</t>
+  </si>
+  <si>
+    <t>oxygen atoms</t>
+  </si>
+  <si>
+    <t>carbon atomes</t>
+  </si>
+  <si>
+    <t>bonds</t>
+  </si>
+  <si>
+    <t>The self-linking ability of carbon is called</t>
+  </si>
+  <si>
+    <t>catenation</t>
+  </si>
+  <si>
+    <t>sublimation</t>
+  </si>
+  <si>
+    <t>hydrogenation</t>
+  </si>
+  <si>
+    <t>carbonation</t>
+  </si>
+  <si>
+    <t>Almost 95% of compounds are of carbon because they can form</t>
+  </si>
+  <si>
+    <t>single bonds</t>
+  </si>
+  <si>
+    <t>double bonds</t>
+  </si>
+  <si>
+    <t>triple bonds</t>
+  </si>
+  <si>
+    <t>multiple bonds</t>
+  </si>
+  <si>
+    <t>Formic acid is also called</t>
+  </si>
+  <si>
+    <t>ethanoic acid</t>
+  </si>
+  <si>
+    <t>methanoic acid</t>
+  </si>
+  <si>
+    <t>carboxylic acid</t>
+  </si>
+  <si>
+    <t>acetone</t>
+  </si>
+  <si>
+    <t>How many isomers are contained by Hexane?</t>
+  </si>
+  <si>
+    <t>two</t>
+  </si>
+  <si>
+    <t>three</t>
+  </si>
+  <si>
+    <t>four</t>
+  </si>
+  <si>
+    <t>five</t>
+  </si>
+  <si>
+    <t>Natural gas mostly consists of</t>
+  </si>
+  <si>
+    <t>ethane</t>
+  </si>
+  <si>
+    <t>butane</t>
+  </si>
+  <si>
+    <t>methane</t>
+  </si>
+  <si>
+    <t>pentane</t>
+  </si>
+  <si>
+    <t>Which of the following is used for artificial ripening of fruits?</t>
+  </si>
+  <si>
+    <t>ethylene</t>
+  </si>
+  <si>
+    <t>acetylene</t>
+  </si>
+  <si>
+    <t>phenol</t>
+  </si>
+  <si>
+    <t>methanol</t>
+  </si>
+  <si>
+    <t>How many bonding electrons are present in the valence shell of carbon?</t>
+  </si>
+  <si>
+    <t>exam duration (in seconds)</t>
   </si>
 </sst>
 </file>
@@ -410,13 +542,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2987332-7617-48E5-9347-AE6CCB924E2C}">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="54.88671875" customWidth="1"/>
+    <col min="4" max="4" width="15.5546875" customWidth="1"/>
+    <col min="5" max="5" width="18.109375" customWidth="1"/>
+    <col min="6" max="6" width="17.109375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -440,19 +578,19 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2">
-        <v>2</v>
-      </c>
-      <c r="F2">
-        <v>3</v>
-      </c>
-      <c r="G2">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -463,23 +601,208 @@
         <v>4</v>
       </c>
       <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" t="s">
+        <v>27</v>
+      </c>
+      <c r="F6" t="s">
+        <v>28</v>
+      </c>
+      <c r="G6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" t="s">
+        <v>32</v>
+      </c>
+      <c r="E7" t="s">
+        <v>31</v>
+      </c>
+      <c r="F7" t="s">
+        <v>33</v>
+      </c>
+      <c r="G7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8">
         <v>7</v>
       </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3">
-        <v>2</v>
-      </c>
-      <c r="F3">
-        <v>3</v>
-      </c>
-      <c r="G3">
-        <v>4</v>
+      <c r="B8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D8" t="s">
+        <v>36</v>
+      </c>
+      <c r="E8" t="s">
+        <v>37</v>
+      </c>
+      <c r="F8" t="s">
+        <v>38</v>
+      </c>
+      <c r="G8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" t="s">
+        <v>40</v>
+      </c>
+      <c r="D9" t="s">
+        <v>41</v>
+      </c>
+      <c r="E9" t="s">
+        <v>42</v>
+      </c>
+      <c r="F9" t="s">
+        <v>43</v>
+      </c>
+      <c r="G9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" t="s">
+        <v>45</v>
+      </c>
+      <c r="D10" t="s">
+        <v>46</v>
+      </c>
+      <c r="E10" t="s">
+        <v>47</v>
+      </c>
+      <c r="F10" t="s">
+        <v>48</v>
+      </c>
+      <c r="G10" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" t="s">
+        <v>50</v>
+      </c>
+      <c r="D11" t="s">
+        <v>36</v>
+      </c>
+      <c r="E11" t="s">
+        <v>37</v>
+      </c>
+      <c r="F11" t="s">
+        <v>38</v>
+      </c>
+      <c r="G11" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -488,22 +811,22 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.44140625" customWidth="1"/>
+    <col min="1" max="1" width="23.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>5</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>10</v>
+        <v>600</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Allow screenshot interval to be read from config
</commit_message>
<xml_diff>
--- a/prototype/sample_questions.xlsx
+++ b/prototype/sample_questions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ca35025d8a608f25/Documents/cs3103proj_exam/prototype/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="99" documentId="8_{3911BD6C-A5DC-4653-B6C0-B36186FF75DF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{832D4618-BC5D-4578-AAA6-C7B709B400C5}"/>
+  <xr:revisionPtr revIDLastSave="106" documentId="8_{3911BD6C-A5DC-4653-B6C0-B36186FF75DF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{055669D0-1B4E-4CD2-863F-5CB3AE4B6526}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B39240BB-16A0-4C86-9AA4-FBD9078AD770}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{B39240BB-16A0-4C86-9AA4-FBD9078AD770}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="53">
   <si>
     <t>No.</t>
   </si>
@@ -191,6 +191,9 @@
   </si>
   <si>
     <t>exam duration (in seconds)</t>
+  </si>
+  <si>
+    <t>Screenshot interval (in seconds)</t>
   </si>
 </sst>
 </file>
@@ -544,7 +547,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2987332-7617-48E5-9347-AE6CCB924E2C}">
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
@@ -808,25 +811,32 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDDA4409-2F4C-4C5D-B9F4-9B8499C90276}">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="23.33203125" customWidth="1"/>
+    <col min="2" max="2" width="32.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>600</v>
+      </c>
+      <c r="B2">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>